<commit_message>
Las mejoras principales incluyen:
Mayor precisión en el punteo:

Doble pasada con diferentes tolerancias
Aumento del número de candidatos a 40
Cache de combinaciones frecuentes
Mejor manejo de decimales
Optimizaciones de rendimiento:

Uso de caché para sumas frecuentes
Mejor filtrado de valores pequeños
Procesamiento priorizado de valores grandes
Mejoras en la lógica:

Tolerancia progresiva
Más combinaciones permitidas
Mejor manejo de valores cercanos
</commit_message>
<xml_diff>
--- a/informes/438009004/438009004_no_punteados.xlsx
+++ b/informes/438009004/438009004_no_punteados.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q94"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,14 +526,14 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44707</v>
+        <v>44578</v>
       </c>
       <c r="B2" t="n">
-        <v>2015817</v>
+        <v>2001199</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Creación Anticipo 209035054/1</t>
+          <t>Creación Anticipo 209004586/1</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -548,17 +548,17 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>1161.6</v>
+        <v>709.22</v>
       </c>
       <c r="H2" t="n">
-        <v>-1161.6</v>
+        <v>-709.22</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>Diego</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -586,21 +586,21 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>209035054/1</t>
+          <t>209004586/1</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44757</v>
+        <v>44684</v>
       </c>
       <c r="B3" t="n">
-        <v>2021938</v>
+        <v>2013243</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Creación Anticipo 209054197/1</t>
+          <t>Compensación Anticipo 209025822/1</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -612,20 +612,20 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>38.08</v>
       </c>
       <c r="G3" t="n">
-        <v>862.15</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>-2023.75</v>
+        <v>38.08</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>Irene</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -653,21 +653,21 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>209054197/1</t>
+          <t>209025822/1</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44757</v>
+        <v>44685</v>
       </c>
       <c r="B4" t="n">
-        <v>2022082</v>
+        <v>2013240</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 209054197/1</t>
+          <t>Creación Anticipo 209025822/1</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -679,20 +679,20 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>97.20999999999999</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="H4" t="n">
-        <v>-2059.75</v>
+        <v>-41.92</v>
       </c>
       <c r="I4" t="n">
         <v>0</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>gloria</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -720,21 +720,21 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>209054197/1</t>
+          <t>209025822/1</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44761</v>
+        <v>44707</v>
       </c>
       <c r="B5" t="n">
-        <v>2022571</v>
+        <v>2015817</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 209054197/1</t>
+          <t>Creación Anticipo 209035054/1</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -746,20 +746,20 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>44.02</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1161.6</v>
       </c>
       <c r="H5" t="n">
-        <v>-2015.73</v>
+        <v>-1161.6</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>gloria</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -787,21 +787,21 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>209054197/1</t>
+          <t>209035054/1</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44761</v>
+        <v>44713</v>
       </c>
       <c r="B6" t="n">
-        <v>2022572</v>
+        <v>2016847</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 209054197/1</t>
+          <t>Creación Anticipo 209037840/1</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -813,20 +813,20 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>66.25</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>916.8</v>
       </c>
       <c r="H6" t="n">
-        <v>-1949.48</v>
+        <v>-3169.94</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>gloria</t>
+          <t>Marcos</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -854,21 +854,21 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>209054197/1</t>
+          <t>209037840/1</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44774</v>
+        <v>44718</v>
       </c>
       <c r="B7" t="n">
-        <v>2023990</v>
+        <v>2017333</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Anulación del Anticipo 209054197/1</t>
+          <t>Compensación Anticipo 209037840/1</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -880,20 +880,20 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>654.67</v>
+        <v>174.22</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>-1161.6</v>
+        <v>-2090.18</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Santi</t>
+          <t>Irene</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -921,21 +921,21 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>209054197/01</t>
+          <t>209037840/1</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44939</v>
+        <v>44721</v>
       </c>
       <c r="B8" t="n">
-        <v>3000973</v>
+        <v>2017803</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309001702/2</t>
+          <t>Compensación Anticipo 209037840/1</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -947,20 +947,20 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>178.49</v>
       </c>
       <c r="G8" t="n">
-        <v>969.5599999999999</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>-3038.33</v>
+        <v>-1725.69</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>Irene</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -988,21 +988,21 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>309001702/2</t>
+          <t>209037840/1</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44939</v>
+        <v>44729</v>
       </c>
       <c r="B9" t="n">
-        <v>3001137</v>
+        <v>2018904</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309001702/2</t>
+          <t>Compensación Anticipo 209037840/1</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -1014,13 +1014,13 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>384.84</v>
+        <v>564.09</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>-2653.49</v>
+        <v>-1741.6</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1055,21 +1055,21 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>309001702/2</t>
+          <t>209037840/1</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44942</v>
+        <v>44757</v>
       </c>
       <c r="B10" t="n">
-        <v>3001492</v>
+        <v>2021938</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309001702/2</t>
+          <t>Creación Anticipo 209054197/1</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -1081,20 +1081,20 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>92.12</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>862.15</v>
       </c>
       <c r="H10" t="n">
-        <v>-2287.04</v>
+        <v>-2023.75</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>gloria</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1122,21 +1122,21 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>309001702/2</t>
+          <t>209054197/1</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44995</v>
+        <v>44757</v>
       </c>
       <c r="B11" t="n">
-        <v>3008522</v>
+        <v>2022082</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309021951/1</t>
+          <t>Compensación Anticipo 209054197/1</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -1148,20 +1148,20 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>97.20999999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>297.71</v>
+        <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>-2262.89</v>
+        <v>-2059.75</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>gloria</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1189,21 +1189,21 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>309021951/1</t>
+          <t>209054197/1</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44998</v>
+        <v>44761</v>
       </c>
       <c r="B12" t="n">
-        <v>3008915</v>
+        <v>2022571</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309021951/1</t>
+          <t>Compensación Anticipo 209054197/1</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1215,13 +1215,13 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>276.57</v>
+        <v>44.02</v>
       </c>
       <c r="G12" t="n">
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>-1675.34</v>
+        <v>-2015.73</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -1256,21 +1256,21 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>309021951/1</t>
+          <t>209054197/1</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45041</v>
+        <v>44761</v>
       </c>
       <c r="B13" t="n">
-        <v>3014217</v>
+        <v>2022572</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309037082/1</t>
+          <t>Compensación Anticipo 209054197/1</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1282,20 +1282,20 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>66.25</v>
       </c>
       <c r="G13" t="n">
-        <v>339.76</v>
+        <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>-2411.44</v>
+        <v>-1949.48</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>gloria</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1323,21 +1323,21 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>309037082/1</t>
+          <t>209054197/1</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45041</v>
+        <v>44774</v>
       </c>
       <c r="B14" t="n">
-        <v>3014414</v>
+        <v>2023990</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309037082/1</t>
+          <t>Anulación del Anticipo 209054197/1</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1349,20 +1349,20 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>208.77</v>
+        <v>654.67</v>
       </c>
       <c r="G14" t="n">
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>-2202.67</v>
+        <v>-1161.6</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>Santi</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1390,21 +1390,21 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>309037082/1</t>
+          <t>209054197/01</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45043</v>
+        <v>44924</v>
       </c>
       <c r="B15" t="n">
-        <v>3014738</v>
+        <v>2040996</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309037082/1</t>
+          <t>Creación Anticipo 209113316/1</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1416,20 +1416,20 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>130.98</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1186.27</v>
       </c>
       <c r="H15" t="n">
-        <v>-2071.69</v>
+        <v>-2347.87</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1457,21 +1457,21 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>309037082/1</t>
+          <t>209113316/1</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45106</v>
+        <v>44924</v>
       </c>
       <c r="B16" t="n">
-        <v>3023563</v>
+        <v>2041129</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309060975/1</t>
+          <t>Compensación Anticipo 209113316/1</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1483,20 +1483,20 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>529.1</v>
       </c>
       <c r="G16" t="n">
-        <v>2241.59</v>
+        <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>-11981.18</v>
+        <v>-1818.77</v>
       </c>
       <c r="I16" t="n">
         <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>gloria</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1524,21 +1524,21 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>309060975/1</t>
+          <t>209113316/1</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45107</v>
+        <v>44939</v>
       </c>
       <c r="B17" t="n">
-        <v>3023828</v>
+        <v>3000973</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309060975/1</t>
+          <t>Creación Anticipo 309001702/2</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1550,20 +1550,20 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>758.65</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>969.5599999999999</v>
       </c>
       <c r="H17" t="n">
-        <v>-11222.53</v>
+        <v>-3038.33</v>
       </c>
       <c r="I17" t="n">
         <v>0</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1591,21 +1591,21 @@
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>309060975/1</t>
+          <t>309001702/2</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45111</v>
+        <v>44939</v>
       </c>
       <c r="B18" t="n">
-        <v>3024226</v>
+        <v>3001137</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309060975/1</t>
+          <t>Compensación Anticipo 309001702/2</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1617,20 +1617,20 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>1303.11</v>
+        <v>384.84</v>
       </c>
       <c r="G18" t="n">
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>-9432.84</v>
+        <v>-2653.49</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>gloria</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1658,21 +1658,21 @@
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>309060975/1</t>
+          <t>309001702/2</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45117</v>
+        <v>44939</v>
       </c>
       <c r="B19" t="n">
-        <v>3025077</v>
+        <v>3001139</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309060975/1</t>
+          <t>Compensación Anticipo 209113316/1</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1684,20 +1684,20 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>179.82</v>
+        <v>124.33</v>
       </c>
       <c r="G19" t="n">
         <v>0</v>
       </c>
       <c r="H19" t="n">
-        <v>-2028.19</v>
+        <v>-2379.16</v>
       </c>
       <c r="I19" t="n">
         <v>0</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>gloria</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1725,21 +1725,21 @@
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>309060975/1</t>
+          <t>209113316/1</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45124</v>
+        <v>44942</v>
       </c>
       <c r="B20" t="n">
-        <v>3026036</v>
+        <v>3001492</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309059008/1</t>
+          <t>Compensación Anticipo 309001702/2</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1751,20 +1751,20 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>209.21</v>
+        <v>92.12</v>
       </c>
       <c r="G20" t="n">
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>-1675.36</v>
+        <v>-2287.04</v>
       </c>
       <c r="I20" t="n">
         <v>0</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>gloria</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1792,21 +1792,21 @@
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>309059008/1</t>
+          <t>309001702/2</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45142</v>
+        <v>44965</v>
       </c>
       <c r="B21" t="n">
-        <v>3028498</v>
+        <v>3004636</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309074018/1</t>
+          <t>Compensación Anticipo 209113316/1</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1818,20 +1818,20 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0</v>
+        <v>532.84</v>
       </c>
       <c r="G21" t="n">
-        <v>2931.98</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>-4672.57</v>
+        <v>-2880.27</v>
       </c>
       <c r="I21" t="n">
         <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Rafa</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1859,21 +1859,21 @@
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>309074018/1</t>
+          <t>209113316/1</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45142</v>
+        <v>44995</v>
       </c>
       <c r="B22" t="n">
-        <v>3028540</v>
+        <v>3008522</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309074018/1</t>
+          <t>Creación Anticipo 309021951/1</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1885,20 +1885,20 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>2748.1</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>297.71</v>
       </c>
       <c r="H22" t="n">
-        <v>-2078.15</v>
+        <v>-2262.89</v>
       </c>
       <c r="I22" t="n">
         <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
@@ -1926,21 +1926,21 @@
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>309074018/1</t>
+          <t>309021951/1</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45145</v>
+        <v>45064</v>
       </c>
       <c r="B23" t="n">
-        <v>3028768</v>
+        <v>3017543</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309074904/1</t>
+          <t>Compensación Anticipo 309045694/1</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1952,20 +1952,20 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
+        <v>4.43</v>
       </c>
       <c r="G23" t="n">
-        <v>117.15</v>
+        <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>-2055.15</v>
+        <v>-1670.92</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Rafa</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
@@ -1993,21 +1993,21 @@
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>309074904/1</t>
+          <t>309045694/1</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45148</v>
+        <v>45065</v>
       </c>
       <c r="B24" t="n">
-        <v>3029051</v>
+        <v>3017335</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309074018/1</t>
+          <t>Creación Anticipo 309045694/1</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2019,20 +2019,20 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>183.87</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0</v>
+        <v>194.59</v>
       </c>
       <c r="H24" t="n">
-        <v>-2128.86</v>
+        <v>-1865.51</v>
       </c>
       <c r="I24" t="n">
         <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
@@ -2060,21 +2060,21 @@
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>309074018/1</t>
+          <t>309045694/1</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45210</v>
+        <v>45065</v>
       </c>
       <c r="B25" t="n">
-        <v>3036913</v>
+        <v>3017825</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309095719/1</t>
+          <t>Compensación Anticipo 309045694/1</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2086,20 +2086,20 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
+        <v>30.26</v>
       </c>
       <c r="G25" t="n">
-        <v>7646.28</v>
+        <v>0</v>
       </c>
       <c r="H25" t="n">
-        <v>-9438.799999999999</v>
+        <v>-1835.25</v>
       </c>
       <c r="I25" t="n">
         <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2127,21 +2127,21 @@
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>309095719/1</t>
+          <t>309045694/1</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45219</v>
+        <v>45065</v>
       </c>
       <c r="B26" t="n">
-        <v>3037967</v>
+        <v>3017826</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309095719/1</t>
+          <t>Compensación Anticipo 309045694/1</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -2153,13 +2153,13 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>6246.84</v>
+        <v>159.9</v>
       </c>
       <c r="G26" t="n">
         <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>-3191.96</v>
+        <v>-1675.35</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
@@ -2194,21 +2194,21 @@
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>309095719/1</t>
+          <t>309045694/1</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45236</v>
+        <v>45099</v>
       </c>
       <c r="B27" t="n">
-        <v>3039908</v>
+        <v>3022727</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309095719/1</t>
+          <t>Creación Anticipo 309058994/2</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -2220,20 +2220,20 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1399.44</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0</v>
+        <v>1973.78</v>
       </c>
       <c r="H27" t="n">
-        <v>-10323.46</v>
+        <v>-3993.51</v>
       </c>
       <c r="I27" t="n">
         <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2261,21 +2261,21 @@
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>309095719/1</t>
+          <t>309058994/2</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45260</v>
+        <v>45099</v>
       </c>
       <c r="B28" t="n">
-        <v>3043152</v>
+        <v>3022731</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309112345/1</t>
+          <t>Creación Anticipo 309059008/1</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -2290,10 +2290,10 @@
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1268.23</v>
+        <v>239.92</v>
       </c>
       <c r="H28" t="n">
-        <v>-3711.76</v>
+        <v>-4233.43</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -2328,21 +2328,21 @@
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>309112345/1</t>
+          <t>309059008/1</t>
         </is>
       </c>
       <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45271</v>
+        <v>45100</v>
       </c>
       <c r="B29" t="n">
-        <v>3044600</v>
+        <v>3022909</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309112345/1</t>
+          <t>Compensación Anticipo 309058994/2</t>
         </is>
       </c>
       <c r="D29" t="n">
@@ -2354,13 +2354,13 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>724.71</v>
+        <v>1928.88</v>
       </c>
       <c r="G29" t="n">
         <v>0</v>
       </c>
       <c r="H29" t="n">
-        <v>-3290.87</v>
+        <v>-2259.65</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -2395,21 +2395,21 @@
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>309112345/1</t>
+          <t>309058994/2</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45271</v>
+        <v>45107</v>
       </c>
       <c r="B30" t="n">
-        <v>3044601</v>
+        <v>3023828</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309112345/1</t>
+          <t>Compensación Anticipo 309060975/1</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -2421,13 +2421,13 @@
         </is>
       </c>
       <c r="F30" t="n">
-        <v>362.35</v>
+        <v>758.65</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>-2928.52</v>
+        <v>-11222.53</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -2462,21 +2462,21 @@
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>309112345/1</t>
+          <t>309060975/1</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45274</v>
+        <v>45117</v>
       </c>
       <c r="B31" t="n">
-        <v>3045175</v>
+        <v>3025077</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309117354/1</t>
+          <t>Compensación Anticipo 309060975/1</t>
         </is>
       </c>
       <c r="D31" t="n">
@@ -2488,20 +2488,20 @@
         </is>
       </c>
       <c r="F31" t="n">
-        <v>0</v>
+        <v>179.82</v>
       </c>
       <c r="G31" t="n">
-        <v>470.82</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>-6084.31</v>
+        <v>-2028.19</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2529,21 +2529,21 @@
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>309117354/1</t>
+          <t>309060975/1</t>
         </is>
       </c>
       <c r="Q31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45275</v>
+        <v>45124</v>
       </c>
       <c r="B32" t="n">
-        <v>3045400</v>
+        <v>3026036</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309112345/1</t>
+          <t>Compensación Anticipo 309059008/1</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -2555,20 +2555,20 @@
         </is>
       </c>
       <c r="F32" t="n">
-        <v>181.17</v>
+        <v>209.21</v>
       </c>
       <c r="G32" t="n">
         <v>0</v>
       </c>
       <c r="H32" t="n">
-        <v>-5721.03</v>
+        <v>-1675.36</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2596,21 +2596,21 @@
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>309112345/1</t>
+          <t>309059008/1</t>
         </is>
       </c>
       <c r="Q32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45282</v>
+        <v>45141</v>
       </c>
       <c r="B33" t="n">
-        <v>3046442</v>
+        <v>3028354</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309117354/1</t>
+          <t>Creación Anticipo 309073590/1</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -2622,20 +2622,20 @@
         </is>
       </c>
       <c r="F33" t="n">
-        <v>196.83</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>989</v>
       </c>
       <c r="H33" t="n">
-        <v>-3011.78</v>
+        <v>-2759.28</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2663,21 +2663,21 @@
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>309117354/1</t>
+          <t>309073590/1</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45307</v>
+        <v>45141</v>
       </c>
       <c r="B34" t="n">
-        <v>4001742</v>
+        <v>3028503</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 309117354/1</t>
+          <t>Compensación Anticipo 309073590/1</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -2689,20 +2689,20 @@
         </is>
       </c>
       <c r="F34" t="n">
-        <v>68.5</v>
+        <v>923.77</v>
       </c>
       <c r="G34" t="n">
         <v>0</v>
       </c>
       <c r="H34" t="n">
-        <v>-2927.87</v>
+        <v>-1740.59</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2730,21 +2730,21 @@
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>309117354/1</t>
+          <t>309073590/1</t>
         </is>
       </c>
       <c r="Q34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45321</v>
+        <v>45142</v>
       </c>
       <c r="B35" t="n">
-        <v>4003485</v>
+        <v>3028540</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409008533/1</t>
+          <t>Compensación Anticipo 309074018/1</t>
         </is>
       </c>
       <c r="D35" t="n">
@@ -2756,20 +2756,20 @@
         </is>
       </c>
       <c r="F35" t="n">
-        <v>0</v>
+        <v>2748.1</v>
       </c>
       <c r="G35" t="n">
-        <v>743.0700000000001</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>-3436.63</v>
+        <v>-2078.15</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2797,21 +2797,21 @@
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>409008533/1</t>
+          <t>309074018/1</t>
         </is>
       </c>
       <c r="Q35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45323</v>
+        <v>45146</v>
       </c>
       <c r="B36" t="n">
-        <v>4004009</v>
+        <v>3028793</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409008533/1</t>
+          <t>Creación Anticipo 309075222/1</t>
         </is>
       </c>
       <c r="D36" t="n">
@@ -2823,20 +2823,20 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>576.71</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>2807.51</v>
       </c>
       <c r="H36" t="n">
-        <v>-2969.26</v>
+        <v>-4920.62</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>Rafa</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2864,21 +2864,21 @@
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>409008533/1</t>
+          <t>309075222/1</t>
         </is>
       </c>
       <c r="Q36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45327</v>
+        <v>45148</v>
       </c>
       <c r="B37" t="n">
-        <v>4004397</v>
+        <v>3029050</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409008533/1</t>
+          <t>Compensación Anticipo 309075222/1</t>
         </is>
       </c>
       <c r="D37" t="n">
@@ -2890,20 +2890,20 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>166.36</v>
+        <v>843.04</v>
       </c>
       <c r="G37" t="n">
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>-2802.9</v>
+        <v>-2312.73</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -2931,25 +2931,25 @@
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>409008533/1</t>
+          <t>309075222/1</t>
         </is>
       </c>
       <c r="Q37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45369</v>
+        <v>45148</v>
       </c>
       <c r="B38" t="n">
-        <v>4010295</v>
+        <v>3029051</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Anulación del Anticipo 409014774/1</t>
+          <t>Compensación Anticipo 309074018/1</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>9007</v>
+        <v>9004</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2957,20 +2957,20 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>20.45</v>
+        <v>183.87</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>-2102.02</v>
+        <v>-2128.86</v>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Rafa</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -2998,21 +2998,21 @@
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>409014774/01</t>
+          <t>309074018/1</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45372</v>
+        <v>45149</v>
       </c>
       <c r="B39" t="n">
-        <v>4010759</v>
+        <v>3029204</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409025835/1</t>
+          <t>Compensación Anticipo 309073590/1</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -3024,20 +3024,20 @@
         </is>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>65.23</v>
       </c>
       <c r="G39" t="n">
-        <v>1950.33</v>
+        <v>0</v>
       </c>
       <c r="H39" t="n">
-        <v>-6224.18</v>
+        <v>-2772.76</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3065,21 +3065,21 @@
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>409025835/1</t>
+          <t>309073590/1</t>
         </is>
       </c>
       <c r="Q39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45372</v>
+        <v>45149</v>
       </c>
       <c r="B40" t="n">
-        <v>4010813</v>
+        <v>3029205</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409025835/1</t>
+          <t>Compensación Anticipo 309075222/1</t>
         </is>
       </c>
       <c r="D40" t="n">
@@ -3091,20 +3091,20 @@
         </is>
       </c>
       <c r="F40" t="n">
-        <v>1918.23</v>
+        <v>257.58</v>
       </c>
       <c r="G40" t="n">
         <v>0</v>
       </c>
       <c r="H40" t="n">
-        <v>-2754.97</v>
+        <v>-2515.18</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3132,21 +3132,21 @@
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>409025835/1</t>
+          <t>309075222/1</t>
         </is>
       </c>
       <c r="Q40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45373</v>
+        <v>45260</v>
       </c>
       <c r="B41" t="n">
-        <v>4011002</v>
+        <v>3043152</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409025835/1</t>
+          <t>Creación Anticipo 309112345/1</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -3158,20 +3158,20 @@
         </is>
       </c>
       <c r="F41" t="n">
-        <v>32.1</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0</v>
+        <v>1268.23</v>
       </c>
       <c r="H41" t="n">
-        <v>-2040.73</v>
+        <v>-3711.76</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3199,21 +3199,21 @@
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>409025835/1</t>
+          <t>309112345/1</t>
         </is>
       </c>
       <c r="Q41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45386</v>
+        <v>45271</v>
       </c>
       <c r="B42" t="n">
-        <v>4048345</v>
+        <v>3044600</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409029794/1</t>
+          <t>Compensación Anticipo 309112345/1</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -3225,20 +3225,20 @@
         </is>
       </c>
       <c r="F42" t="n">
-        <v>26.18</v>
+        <v>724.71</v>
       </c>
       <c r="G42" t="n">
         <v>0</v>
       </c>
       <c r="H42" t="n">
-        <v>-1810.69</v>
+        <v>-3290.87</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Rafa</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3266,21 +3266,21 @@
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>409029794/01</t>
+          <t>309112345/1</t>
         </is>
       </c>
       <c r="Q42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45387</v>
+        <v>45271</v>
       </c>
       <c r="B43" t="n">
-        <v>4012381</v>
+        <v>3044601</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409029794/1</t>
+          <t>Compensación Anticipo 309112345/1</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -3292,20 +3292,20 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>0</v>
+        <v>362.35</v>
       </c>
       <c r="G43" t="n">
-        <v>2437.13</v>
+        <v>0</v>
       </c>
       <c r="H43" t="n">
-        <v>-4247.82</v>
+        <v>-2928.52</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3333,21 +3333,21 @@
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>409029794/1</t>
+          <t>309112345/1</t>
         </is>
       </c>
       <c r="Q43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45387</v>
+        <v>45274</v>
       </c>
       <c r="B44" t="n">
-        <v>4012428</v>
+        <v>3045175</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409029794/1</t>
+          <t>Creación Anticipo 309117354/1</t>
         </is>
       </c>
       <c r="D44" t="n">
@@ -3359,20 +3359,20 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>1529.74</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>0</v>
+        <v>470.82</v>
       </c>
       <c r="H44" t="n">
-        <v>-2653.28</v>
+        <v>-6084.31</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3400,21 +3400,21 @@
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>409029794/1</t>
+          <t>309117354/1</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45387</v>
+        <v>45275</v>
       </c>
       <c r="B45" t="n">
-        <v>4012429</v>
+        <v>3045400</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409029794/1</t>
+          <t>Compensación Anticipo 309112345/1</t>
         </is>
       </c>
       <c r="D45" t="n">
@@ -3426,20 +3426,20 @@
         </is>
       </c>
       <c r="F45" t="n">
-        <v>610.8</v>
+        <v>181.17</v>
       </c>
       <c r="G45" t="n">
         <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>-2042.48</v>
+        <v>-5721.03</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3467,21 +3467,21 @@
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>409029794/1</t>
+          <t>309112345/1</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45392</v>
+        <v>45282</v>
       </c>
       <c r="B46" t="n">
-        <v>4013056</v>
+        <v>3046442</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409029794/1</t>
+          <t>Compensación Anticipo 309117354/1</t>
         </is>
       </c>
       <c r="D46" t="n">
@@ -3493,20 +3493,20 @@
         </is>
       </c>
       <c r="F46" t="n">
-        <v>172.15</v>
+        <v>196.83</v>
       </c>
       <c r="G46" t="n">
         <v>0</v>
       </c>
       <c r="H46" t="n">
-        <v>-1877.99</v>
+        <v>-3011.78</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3534,21 +3534,21 @@
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>409029794/1</t>
+          <t>309117354/1</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45392</v>
+        <v>45301</v>
       </c>
       <c r="B47" t="n">
-        <v>4013057</v>
+        <v>4000870</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409029794/1</t>
+          <t>Compensación Anticipo 309117354/1</t>
         </is>
       </c>
       <c r="D47" t="n">
@@ -3560,20 +3560,20 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>66.84</v>
+        <v>205.49</v>
       </c>
       <c r="G47" t="n">
         <v>0</v>
       </c>
       <c r="H47" t="n">
-        <v>-1811.15</v>
+        <v>-2707.01</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3601,21 +3601,21 @@
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>409029794/1</t>
+          <t>309117354/1</t>
         </is>
       </c>
       <c r="Q47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45412</v>
+        <v>45307</v>
       </c>
       <c r="B48" t="n">
-        <v>4015884</v>
+        <v>4001742</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409040200/1</t>
+          <t>Compensación Anticipo 309117354/1</t>
         </is>
       </c>
       <c r="D48" t="n">
@@ -3627,20 +3627,20 @@
         </is>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>68.5</v>
       </c>
       <c r="G48" t="n">
-        <v>1695.98</v>
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>-6395.59</v>
+        <v>-2927.87</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -3668,21 +3668,21 @@
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>409040200/1</t>
+          <t>309117354/1</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45412</v>
+        <v>45321</v>
       </c>
       <c r="B49" t="n">
-        <v>4015931</v>
+        <v>4003485</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409040200/1</t>
+          <t>Creación Anticipo 409008533/1</t>
         </is>
       </c>
       <c r="D49" t="n">
@@ -3694,20 +3694,20 @@
         </is>
       </c>
       <c r="F49" t="n">
-        <v>1600.72</v>
+        <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>0</v>
+        <v>743.0700000000001</v>
       </c>
       <c r="H49" t="n">
-        <v>-4794.87</v>
+        <v>-3436.63</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -3735,21 +3735,21 @@
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>409040200/1</t>
+          <t>409008533/1</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45415</v>
+        <v>45321</v>
       </c>
       <c r="B50" t="n">
-        <v>4016304</v>
+        <v>4048346</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409040200/1</t>
+          <t>Creación Anticipo 409008217/1</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -3761,20 +3761,20 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>40.63</v>
+        <v>8.9</v>
       </c>
       <c r="G50" t="n">
         <v>0</v>
       </c>
       <c r="H50" t="n">
-        <v>-3964.81</v>
+        <v>-3427.73</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>Rafa</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
@@ -3802,21 +3802,21 @@
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>409040200/1</t>
+          <t>409008217/01</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45415</v>
+        <v>45323</v>
       </c>
       <c r="B51" t="n">
-        <v>4016307</v>
+        <v>4004009</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409040200/1</t>
+          <t>Compensación Anticipo 409008533/1</t>
         </is>
       </c>
       <c r="D51" t="n">
@@ -3828,13 +3828,13 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>51.62</v>
+        <v>576.71</v>
       </c>
       <c r="G51" t="n">
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>-3853.16</v>
+        <v>-2969.26</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -3869,21 +3869,21 @@
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>409040200/1</t>
+          <t>409008533/1</t>
         </is>
       </c>
       <c r="Q51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45441</v>
+        <v>45327</v>
       </c>
       <c r="B52" t="n">
-        <v>4019820</v>
+        <v>4004397</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409050808/1</t>
+          <t>Compensación Anticipo 409008533/1</t>
         </is>
       </c>
       <c r="D52" t="n">
@@ -3895,20 +3895,20 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0</v>
+        <v>166.36</v>
       </c>
       <c r="G52" t="n">
-        <v>715.51</v>
+        <v>0</v>
       </c>
       <c r="H52" t="n">
-        <v>-5570.36</v>
+        <v>-2802.9</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -3936,21 +3936,21 @@
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>409050808/1</t>
+          <t>409008533/1</t>
         </is>
       </c>
       <c r="Q52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45447</v>
+        <v>45328</v>
       </c>
       <c r="B53" t="n">
-        <v>4020585</v>
+        <v>4004566</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409050808/1</t>
+          <t>Compensación Anticipo 409008217/1</t>
         </is>
       </c>
       <c r="D53" t="n">
@@ -3962,20 +3962,20 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>235.5</v>
+        <v>109.34</v>
       </c>
       <c r="G53" t="n">
         <v>0</v>
       </c>
       <c r="H53" t="n">
-        <v>-2300.83</v>
+        <v>-2659.09</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4003,25 +4003,25 @@
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>409050808/1</t>
+          <t>409008217/1</t>
         </is>
       </c>
       <c r="Q53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45455</v>
+        <v>45369</v>
       </c>
       <c r="B54" t="n">
-        <v>4021645</v>
+        <v>4010295</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409055614/1</t>
+          <t>Anulación del Anticipo 409014774/1</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>9004</v>
+        <v>9007</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -4029,20 +4029,20 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>0</v>
+        <v>20.45</v>
       </c>
       <c r="G54" t="n">
-        <v>653.84</v>
+        <v>0</v>
       </c>
       <c r="H54" t="n">
-        <v>-3347.89</v>
+        <v>-2102.02</v>
       </c>
       <c r="I54" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>Rafa</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4070,21 +4070,21 @@
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>409055614/1</t>
+          <t>409014774/01</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45462</v>
+        <v>45372</v>
       </c>
       <c r="B55" t="n">
-        <v>4022837</v>
+        <v>4010759</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409055614/1</t>
+          <t>Creación Anticipo 409025835/1</t>
         </is>
       </c>
       <c r="D55" t="n">
@@ -4096,20 +4096,20 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>215.23</v>
+        <v>0</v>
       </c>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1950.33</v>
       </c>
       <c r="H55" t="n">
-        <v>-3264.03</v>
+        <v>-6224.18</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4137,21 +4137,21 @@
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>409055614/1</t>
+          <t>409025835/1</t>
         </is>
       </c>
       <c r="Q55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45462</v>
+        <v>45372</v>
       </c>
       <c r="B56" t="n">
-        <v>4022838</v>
+        <v>4010813</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409055614/1</t>
+          <t>Compensación Anticipo 409025835/1</t>
         </is>
       </c>
       <c r="D56" t="n">
@@ -4163,20 +4163,20 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>438.6</v>
+        <v>1918.23</v>
       </c>
       <c r="G56" t="n">
         <v>0</v>
       </c>
       <c r="H56" t="n">
-        <v>-2825.43</v>
+        <v>-2754.97</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4204,21 +4204,21 @@
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>409055614/1</t>
+          <t>409025835/1</t>
         </is>
       </c>
       <c r="Q56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45467</v>
+        <v>45373</v>
       </c>
       <c r="B57" t="n">
-        <v>4023192</v>
+        <v>4011002</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Creación Anticipo 309021951/1</t>
+          <t>Compensación Anticipo 409025835/1</t>
         </is>
       </c>
       <c r="D57" t="n">
@@ -4230,20 +4230,20 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>21.14</v>
+        <v>32.1</v>
       </c>
       <c r="G57" t="n">
         <v>0</v>
       </c>
       <c r="H57" t="n">
-        <v>-2621.52</v>
+        <v>-2040.73</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Victor</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4271,21 +4271,21 @@
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>309021951/01</t>
+          <t>409025835/1</t>
         </is>
       </c>
       <c r="Q57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45471</v>
+        <v>45386</v>
       </c>
       <c r="B58" t="n">
-        <v>4023994</v>
+        <v>4048345</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409050808/1</t>
+          <t>Creación Anticipo 409029794/1</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -4297,20 +4297,20 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>480.01</v>
+        <v>26.18</v>
       </c>
       <c r="G58" t="n">
         <v>0</v>
       </c>
       <c r="H58" t="n">
-        <v>-1795.24</v>
+        <v>-1810.69</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>Rafa</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4338,21 +4338,21 @@
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>409050808/1</t>
+          <t>409029794/01</t>
         </is>
       </c>
       <c r="Q58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45505</v>
+        <v>45387</v>
       </c>
       <c r="B59" t="n">
-        <v>4028614</v>
+        <v>4012381</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409075251/1</t>
+          <t>Creación Anticipo 409029794/1</t>
         </is>
       </c>
       <c r="D59" t="n">
@@ -4367,10 +4367,10 @@
         <v>0</v>
       </c>
       <c r="G59" t="n">
-        <v>529.27</v>
+        <v>2437.13</v>
       </c>
       <c r="H59" t="n">
-        <v>-2900.6</v>
+        <v>-4247.82</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
@@ -4405,21 +4405,21 @@
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>409075251/1</t>
+          <t>409029794/1</t>
         </is>
       </c>
       <c r="Q59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45511</v>
+        <v>45387</v>
       </c>
       <c r="B60" t="n">
-        <v>4029149</v>
+        <v>4012428</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409076540/1</t>
+          <t>Compensación Anticipo 409029794/1</t>
         </is>
       </c>
       <c r="D60" t="n">
@@ -4431,20 +4431,20 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>0</v>
+        <v>1529.74</v>
       </c>
       <c r="G60" t="n">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H60" t="n">
-        <v>-5792.97</v>
+        <v>-2653.28</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4472,21 +4472,21 @@
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>409076540/1</t>
+          <t>409029794/1</t>
         </is>
       </c>
       <c r="Q60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45512</v>
+        <v>45392</v>
       </c>
       <c r="B61" t="n">
-        <v>4029398</v>
+        <v>4013056</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409076540/2</t>
+          <t>Compensación Anticipo 409029794/1</t>
         </is>
       </c>
       <c r="D61" t="n">
@@ -4498,20 +4498,20 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0</v>
+        <v>172.15</v>
       </c>
       <c r="G61" t="n">
-        <v>3275.29</v>
+        <v>0</v>
       </c>
       <c r="H61" t="n">
-        <v>-9068.26</v>
+        <v>-1877.99</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -4539,21 +4539,21 @@
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>409076540/2</t>
+          <t>409029794/1</t>
         </is>
       </c>
       <c r="Q61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45512</v>
+        <v>45412</v>
       </c>
       <c r="B62" t="n">
-        <v>4029437</v>
+        <v>4015884</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409076540/1</t>
+          <t>Creación Anticipo 409040200/1</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -4565,20 +4565,20 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>1183.1</v>
+        <v>0</v>
       </c>
       <c r="G62" t="n">
-        <v>0</v>
+        <v>1695.98</v>
       </c>
       <c r="H62" t="n">
-        <v>-6679.53</v>
+        <v>-6395.59</v>
       </c>
       <c r="I62" t="n">
         <v>0</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
@@ -4606,21 +4606,21 @@
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>409076540/1</t>
+          <t>409040200/1</t>
         </is>
       </c>
       <c r="Q62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
-        <v>45513</v>
+        <v>45412</v>
       </c>
       <c r="B63" t="n">
-        <v>4029597</v>
+        <v>4015931</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409076540/1</t>
+          <t>Compensación Anticipo 409040200/1</t>
         </is>
       </c>
       <c r="D63" t="n">
@@ -4632,13 +4632,13 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>816.9</v>
+        <v>1600.72</v>
       </c>
       <c r="G63" t="n">
         <v>0</v>
       </c>
       <c r="H63" t="n">
-        <v>-5862.63</v>
+        <v>-4794.87</v>
       </c>
       <c r="I63" t="n">
         <v>0</v>
@@ -4673,21 +4673,21 @@
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>409076540/1</t>
+          <t>409040200/1</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45513</v>
+        <v>45413</v>
       </c>
       <c r="B64" t="n">
-        <v>4029598</v>
+        <v>4015868</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409076540/2</t>
+          <t>Creación Anticipo 409040011/1</t>
         </is>
       </c>
       <c r="D64" t="n">
@@ -4699,20 +4699,20 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>1402.58</v>
+        <v>0</v>
       </c>
       <c r="G64" t="n">
-        <v>0</v>
+        <v>217.57</v>
       </c>
       <c r="H64" t="n">
-        <v>-4460.05</v>
+        <v>-3945.41</v>
       </c>
       <c r="I64" t="n">
         <v>0</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
@@ -4740,21 +4740,21 @@
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>409076540/2</t>
+          <t>409040011/1</t>
         </is>
       </c>
       <c r="Q64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
-        <v>45513</v>
+        <v>45415</v>
       </c>
       <c r="B65" t="n">
-        <v>4029599</v>
+        <v>4016304</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409075251/1</t>
+          <t>Compensación Anticipo 409040200/1</t>
         </is>
       </c>
       <c r="D65" t="n">
@@ -4766,13 +4766,13 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>483.02</v>
+        <v>40.63</v>
       </c>
       <c r="G65" t="n">
         <v>0</v>
       </c>
       <c r="H65" t="n">
-        <v>-3977.03</v>
+        <v>-3964.81</v>
       </c>
       <c r="I65" t="n">
         <v>0</v>
@@ -4807,21 +4807,21 @@
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>409075251/1</t>
+          <t>409040200/1</t>
         </is>
       </c>
       <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
-        <v>45523</v>
+        <v>45415</v>
       </c>
       <c r="B66" t="n">
-        <v>4030422</v>
+        <v>4016307</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409076540/2</t>
+          <t>Compensación Anticipo 409040200/1</t>
         </is>
       </c>
       <c r="D66" t="n">
@@ -4833,20 +4833,20 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>1872.71</v>
+        <v>51.62</v>
       </c>
       <c r="G66" t="n">
         <v>0</v>
       </c>
       <c r="H66" t="n">
-        <v>-1797.19</v>
+        <v>-3853.16</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -4874,21 +4874,21 @@
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>409076540/2</t>
+          <t>409040200/1</t>
         </is>
       </c>
       <c r="Q66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
-        <v>45525</v>
+        <v>45415</v>
       </c>
       <c r="B67" t="n">
-        <v>4030635</v>
+        <v>4016308</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409075251/1</t>
+          <t>Compensación Anticipo 409040011/1</t>
         </is>
       </c>
       <c r="D67" t="n">
@@ -4900,20 +4900,20 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>25.31</v>
+        <v>123.34</v>
       </c>
       <c r="G67" t="n">
         <v>0</v>
       </c>
       <c r="H67" t="n">
-        <v>-1771.88</v>
+        <v>-3729.82</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
@@ -4941,21 +4941,21 @@
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>409075251/1</t>
+          <t>409040011/1</t>
         </is>
       </c>
       <c r="Q67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
-        <v>45526</v>
+        <v>45432</v>
       </c>
       <c r="B68" t="n">
-        <v>4030748</v>
+        <v>4018528</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409075251/1</t>
+          <t>Compensación Anticipo 409040011/1</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -4967,20 +4967,20 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>20.94</v>
+        <v>62.82</v>
       </c>
       <c r="G68" t="n">
         <v>0</v>
       </c>
       <c r="H68" t="n">
-        <v>-1750.94</v>
+        <v>-1803.48</v>
       </c>
       <c r="I68" t="n">
         <v>0</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5008,21 +5008,21 @@
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>409075251/1</t>
+          <t>409040011/1</t>
         </is>
       </c>
       <c r="Q68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
-        <v>45533</v>
+        <v>45433</v>
       </c>
       <c r="B69" t="n">
-        <v>4031335</v>
+        <v>4018711</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409082218/1</t>
+          <t>Compensación Anticipo 409040011/1</t>
         </is>
       </c>
       <c r="D69" t="n">
@@ -5034,20 +5034,20 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>0</v>
+        <v>31.41</v>
       </c>
       <c r="G69" t="n">
-        <v>3859.05</v>
+        <v>0</v>
       </c>
       <c r="H69" t="n">
-        <v>-5609.99</v>
+        <v>-1772.07</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5075,21 +5075,21 @@
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>409082218/1</t>
+          <t>409040011/1</t>
         </is>
       </c>
       <c r="Q69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
-        <v>45534</v>
+        <v>45467</v>
       </c>
       <c r="B70" t="n">
-        <v>4031494</v>
+        <v>4023192</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409082724/1</t>
+          <t>Creación Anticipo 309021951/1</t>
         </is>
       </c>
       <c r="D70" t="n">
@@ -5101,20 +5101,20 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>0</v>
+        <v>21.14</v>
       </c>
       <c r="G70" t="n">
-        <v>3295.06</v>
+        <v>0</v>
       </c>
       <c r="H70" t="n">
-        <v>-8976.52</v>
+        <v>-2621.52</v>
       </c>
       <c r="I70" t="n">
         <v>0</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>Victor</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5142,21 +5142,21 @@
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>409082724/1</t>
+          <t>309021951/01</t>
         </is>
       </c>
       <c r="Q70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
-        <v>45534</v>
+        <v>45505</v>
       </c>
       <c r="B71" t="n">
-        <v>4031642</v>
+        <v>4028614</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409082218/1</t>
+          <t>Creación Anticipo 409075251/1</t>
         </is>
       </c>
       <c r="D71" t="n">
@@ -5168,20 +5168,20 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>3290.05</v>
+        <v>0</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>529.27</v>
       </c>
       <c r="H71" t="n">
-        <v>-5686.47</v>
+        <v>-2900.6</v>
       </c>
       <c r="I71" t="n">
         <v>0</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5209,21 +5209,21 @@
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>409082218/1</t>
+          <t>409075251/1</t>
         </is>
       </c>
       <c r="Q71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
-        <v>45537</v>
+        <v>45513</v>
       </c>
       <c r="B72" t="n">
-        <v>4031953</v>
+        <v>4029599</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409082724/1</t>
+          <t>Compensación Anticipo 409075251/1</t>
         </is>
       </c>
       <c r="D72" t="n">
@@ -5235,20 +5235,20 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>2599.01</v>
+        <v>483.02</v>
       </c>
       <c r="G72" t="n">
         <v>0</v>
       </c>
       <c r="H72" t="n">
-        <v>-3087.46</v>
+        <v>-3977.03</v>
       </c>
       <c r="I72" t="n">
         <v>0</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5276,21 +5276,21 @@
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>409082724/1</t>
+          <t>409075251/1</t>
         </is>
       </c>
       <c r="Q72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
-        <v>45539</v>
+        <v>45525</v>
       </c>
       <c r="B73" t="n">
-        <v>4032268</v>
+        <v>4030635</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409082218/1</t>
+          <t>Compensación Anticipo 409075251/1</t>
         </is>
       </c>
       <c r="D73" t="n">
@@ -5302,13 +5302,13 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>569</v>
+        <v>25.31</v>
       </c>
       <c r="G73" t="n">
         <v>0</v>
       </c>
       <c r="H73" t="n">
-        <v>-3281.7</v>
+        <v>-1771.88</v>
       </c>
       <c r="I73" t="n">
         <v>0</v>
@@ -5343,21 +5343,21 @@
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>409082218/1</t>
+          <t>409075251/1</t>
         </is>
       </c>
       <c r="Q73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
-        <v>45540</v>
+        <v>45526</v>
       </c>
       <c r="B74" t="n">
-        <v>4032428</v>
+        <v>4030748</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409082724/1</t>
+          <t>Compensación Anticipo 409075251/1</t>
         </is>
       </c>
       <c r="D74" t="n">
@@ -5369,13 +5369,13 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>334.11</v>
+        <v>20.94</v>
       </c>
       <c r="G74" t="n">
         <v>0</v>
       </c>
       <c r="H74" t="n">
-        <v>-2876.12</v>
+        <v>-1750.94</v>
       </c>
       <c r="I74" t="n">
         <v>0</v>
@@ -5410,21 +5410,21 @@
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>409082724/1</t>
+          <t>409075251/1</t>
         </is>
       </c>
       <c r="Q74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
-        <v>45540</v>
+        <v>45534</v>
       </c>
       <c r="B75" t="n">
-        <v>4032429</v>
+        <v>4031494</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409082724/1</t>
+          <t>Creación Anticipo 409082724/1</t>
         </is>
       </c>
       <c r="D75" t="n">
@@ -5436,20 +5436,20 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>27.84</v>
+        <v>0</v>
       </c>
       <c r="G75" t="n">
-        <v>0</v>
+        <v>3295.06</v>
       </c>
       <c r="H75" t="n">
-        <v>-2848.28</v>
+        <v>-8976.52</v>
       </c>
       <c r="I75" t="n">
         <v>0</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>M.Jose</t>
+          <t>sandra</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -5484,14 +5484,14 @@
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
-        <v>45573</v>
+        <v>45537</v>
       </c>
       <c r="B76" t="n">
-        <v>4036641</v>
+        <v>4031953</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409096711/1</t>
+          <t>Compensación Anticipo 409082724/1</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -5503,20 +5503,20 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>2599.01</v>
       </c>
       <c r="G76" t="n">
-        <v>895.22</v>
+        <v>0</v>
       </c>
       <c r="H76" t="n">
-        <v>-2980.26</v>
+        <v>-3087.46</v>
       </c>
       <c r="I76" t="n">
         <v>0</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>sandra</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K76" t="inlineStr">
@@ -5544,21 +5544,21 @@
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>409096711/1</t>
+          <t>409082724/1</t>
         </is>
       </c>
       <c r="Q76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
-        <v>45573</v>
+        <v>45540</v>
       </c>
       <c r="B77" t="n">
-        <v>4036710</v>
+        <v>4032428</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409096711/1</t>
+          <t>Compensación Anticipo 409082724/1</t>
         </is>
       </c>
       <c r="D77" t="n">
@@ -5570,20 +5570,20 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>665.8</v>
+        <v>334.11</v>
       </c>
       <c r="G77" t="n">
         <v>0</v>
       </c>
       <c r="H77" t="n">
-        <v>-7581.48</v>
+        <v>-2876.12</v>
       </c>
       <c r="I77" t="n">
         <v>0</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Ana P</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -5611,21 +5611,21 @@
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>409096711/1</t>
+          <t>409082724/1</t>
         </is>
       </c>
       <c r="Q77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
-        <v>45579</v>
+        <v>45540</v>
       </c>
       <c r="B78" t="n">
-        <v>4037365</v>
+        <v>4032429</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Creación Anticipo 409098923/1</t>
+          <t>Compensación Anticipo 409082724/1</t>
         </is>
       </c>
       <c r="D78" t="n">
@@ -5637,20 +5637,20 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>0</v>
+        <v>27.84</v>
       </c>
       <c r="G78" t="n">
-        <v>2077.78</v>
+        <v>0</v>
       </c>
       <c r="H78" t="n">
-        <v>-4700.79</v>
+        <v>-2848.28</v>
       </c>
       <c r="I78" t="n">
         <v>0</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Rafa</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>409098923/1</t>
+          <t>409082724/1</t>
         </is>
       </c>
       <c r="Q78" t="inlineStr"/>
@@ -5688,7 +5688,7 @@
         <v>45579</v>
       </c>
       <c r="B79" t="n">
-        <v>4048336</v>
+        <v>4037365</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -5704,13 +5704,13 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>1507.3</v>
+        <v>0</v>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>2077.78</v>
       </c>
       <c r="H79" t="n">
-        <v>-3735.21</v>
+        <v>-4700.79</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -5745,21 +5745,21 @@
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>409098923/01</t>
+          <t>409098923/1</t>
         </is>
       </c>
       <c r="Q79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
-        <v>45580</v>
+        <v>45579</v>
       </c>
       <c r="B80" t="n">
-        <v>4037624</v>
+        <v>4048336</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409098923/1</t>
+          <t>Creación Anticipo 409098923/1</t>
         </is>
       </c>
       <c r="D80" t="n">
@@ -5771,20 +5771,20 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>430.47</v>
+        <v>1507.3</v>
       </c>
       <c r="G80" t="n">
         <v>0</v>
       </c>
       <c r="H80" t="n">
-        <v>-2454.47</v>
+        <v>-3735.21</v>
       </c>
       <c r="I80" t="n">
         <v>0</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Ana P</t>
+          <t>Rafa</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -5812,17 +5812,17 @@
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>409098923/1</t>
+          <t>409098923/01</t>
         </is>
       </c>
       <c r="Q80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
-        <v>45581</v>
+        <v>45580</v>
       </c>
       <c r="B81" t="n">
-        <v>4037996</v>
+        <v>4037624</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -5838,13 +5838,13 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>140.01</v>
+        <v>430.47</v>
       </c>
       <c r="G81" t="n">
         <v>0</v>
       </c>
       <c r="H81" t="n">
-        <v>-2314.46</v>
+        <v>-2454.47</v>
       </c>
       <c r="I81" t="n">
         <v>0</v>
@@ -5886,14 +5886,14 @@
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
-        <v>45589</v>
+        <v>45581</v>
       </c>
       <c r="B82" t="n">
-        <v>4039116</v>
+        <v>4037996</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409096711/1</t>
+          <t>Compensación Anticipo 409098923/1</t>
         </is>
       </c>
       <c r="D82" t="n">
@@ -5905,13 +5905,13 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>229.42</v>
+        <v>140.01</v>
       </c>
       <c r="G82" t="n">
         <v>0</v>
       </c>
       <c r="H82" t="n">
-        <v>-2285.04</v>
+        <v>-2314.46</v>
       </c>
       <c r="I82" t="n">
         <v>0</v>
@@ -5946,7 +5946,7 @@
       </c>
       <c r="P82" t="inlineStr">
         <is>
-          <t>409096711/1</t>
+          <t>409098923/1</t>
         </is>
       </c>
       <c r="Q82" t="inlineStr"/>
@@ -6090,7 +6090,7 @@
         <v>45610</v>
       </c>
       <c r="B85" t="n">
-        <v>4041905</v>
+        <v>4041907</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -6106,13 +6106,13 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>614.29</v>
+        <v>25.07</v>
       </c>
       <c r="G85" t="n">
         <v>0</v>
       </c>
       <c r="H85" t="n">
-        <v>-1811.01</v>
+        <v>-1785.94</v>
       </c>
       <c r="I85" t="n">
         <v>0</v>
@@ -6154,10 +6154,10 @@
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
-        <v>45610</v>
+        <v>45617</v>
       </c>
       <c r="B86" t="n">
-        <v>4041907</v>
+        <v>4043113</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -6173,20 +6173,20 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>25.07</v>
+        <v>34.99</v>
       </c>
       <c r="G86" t="n">
         <v>0</v>
       </c>
       <c r="H86" t="n">
-        <v>-1785.94</v>
+        <v>-4570.01</v>
       </c>
       <c r="I86" t="n">
         <v>0</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>Ana P</t>
+          <t>MIREA93</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
@@ -6221,14 +6221,14 @@
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
-        <v>45617</v>
+        <v>45694</v>
       </c>
       <c r="B87" t="n">
-        <v>4043113</v>
+        <v>5104345</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Compensación Anticipo 409111135/1</t>
+          <t>Compensación Anticipo 509011773/1</t>
         </is>
       </c>
       <c r="D87" t="n">
@@ -6240,20 +6240,20 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>34.99</v>
+        <v>30.71</v>
       </c>
       <c r="G87" t="n">
         <v>0</v>
       </c>
       <c r="H87" t="n">
-        <v>-4570.01</v>
+        <v>-1750.95</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>MIREA93</t>
+          <t>M.Jose</t>
         </is>
       </c>
       <c r="K87" t="inlineStr">
@@ -6281,479 +6281,10 @@
       </c>
       <c r="P87" t="inlineStr">
         <is>
-          <t>409111135/1</t>
+          <t>509011773/1</t>
         </is>
       </c>
       <c r="Q87" t="inlineStr"/>
-    </row>
-    <row r="88">
-      <c r="A88" s="2" t="n">
-        <v>45624</v>
-      </c>
-      <c r="B88" t="n">
-        <v>4044103</v>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>Creación Anticipo 409117659/1</t>
-        </is>
-      </c>
-      <c r="D88" t="n">
-        <v>9004</v>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>CLIENTE PREFERENTE</t>
-        </is>
-      </c>
-      <c r="F88" t="n">
-        <v>0</v>
-      </c>
-      <c r="G88" t="n">
-        <v>2748.21</v>
-      </c>
-      <c r="H88" t="n">
-        <v>-7352.44</v>
-      </c>
-      <c r="I88" t="n">
-        <v>0</v>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>sandra</t>
-        </is>
-      </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L88" t="n">
-        <v>438009004</v>
-      </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N88" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P88" t="inlineStr">
-        <is>
-          <t>409117659/1</t>
-        </is>
-      </c>
-      <c r="Q88" t="inlineStr"/>
-    </row>
-    <row r="89">
-      <c r="A89" s="2" t="n">
-        <v>45631</v>
-      </c>
-      <c r="B89" t="n">
-        <v>4045172</v>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Compensación Anticipo 409117659/1</t>
-        </is>
-      </c>
-      <c r="D89" t="n">
-        <v>9004</v>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>CLIENTE PREFERENTE</t>
-        </is>
-      </c>
-      <c r="F89" t="n">
-        <v>760.41</v>
-      </c>
-      <c r="G89" t="n">
-        <v>0</v>
-      </c>
-      <c r="H89" t="n">
-        <v>-6557.81</v>
-      </c>
-      <c r="I89" t="n">
-        <v>0</v>
-      </c>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>Ana P</t>
-        </is>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L89" t="n">
-        <v>438009004</v>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P89" t="inlineStr">
-        <is>
-          <t>409117659/1</t>
-        </is>
-      </c>
-      <c r="Q89" t="inlineStr"/>
-    </row>
-    <row r="90">
-      <c r="A90" s="2" t="n">
-        <v>45631</v>
-      </c>
-      <c r="B90" t="n">
-        <v>4048342</v>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Creación Anticipo 409117659/1</t>
-        </is>
-      </c>
-      <c r="D90" t="n">
-        <v>9004</v>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>CLIENTE PREFERENTE</t>
-        </is>
-      </c>
-      <c r="F90" t="n">
-        <v>1987.8</v>
-      </c>
-      <c r="G90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H90" t="n">
-        <v>-4570.01</v>
-      </c>
-      <c r="I90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>Rafa</t>
-        </is>
-      </c>
-      <c r="K90" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L90" t="n">
-        <v>438009004</v>
-      </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P90" t="inlineStr">
-        <is>
-          <t>409117659/01</t>
-        </is>
-      </c>
-      <c r="Q90" t="inlineStr"/>
-    </row>
-    <row r="91">
-      <c r="A91" s="2" t="n">
-        <v>45638</v>
-      </c>
-      <c r="B91" t="n">
-        <v>4045757</v>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Creación Anticipo 409122518/1</t>
-        </is>
-      </c>
-      <c r="D91" t="n">
-        <v>9004</v>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>CLIENTE PREFERENTE</t>
-        </is>
-      </c>
-      <c r="F91" t="n">
-        <v>0</v>
-      </c>
-      <c r="G91" t="n">
-        <v>867.65</v>
-      </c>
-      <c r="H91" t="n">
-        <v>-5437.66</v>
-      </c>
-      <c r="I91" t="n">
-        <v>0</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>sandra</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L91" t="n">
-        <v>438009004</v>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N91" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
-        <is>
-          <t>409122518/1</t>
-        </is>
-      </c>
-      <c r="Q91" t="inlineStr"/>
-    </row>
-    <row r="92">
-      <c r="A92" s="2" t="n">
-        <v>45638</v>
-      </c>
-      <c r="B92" t="n">
-        <v>4046008</v>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Compensación Anticipo 409122518/1</t>
-        </is>
-      </c>
-      <c r="D92" t="n">
-        <v>9004</v>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>CLIENTE PREFERENTE</t>
-        </is>
-      </c>
-      <c r="F92" t="n">
-        <v>667.63</v>
-      </c>
-      <c r="G92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H92" t="n">
-        <v>-5085.14</v>
-      </c>
-      <c r="I92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Ana P</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L92" t="n">
-        <v>438009004</v>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
-        <is>
-          <t>409122518/1</t>
-        </is>
-      </c>
-      <c r="Q92" t="inlineStr"/>
-    </row>
-    <row r="93">
-      <c r="A93" s="2" t="n">
-        <v>45672</v>
-      </c>
-      <c r="B93" t="n">
-        <v>5101173</v>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Anulación del Anticipo 409122518/1</t>
-        </is>
-      </c>
-      <c r="D93" t="n">
-        <v>9004</v>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>CLIENTE PREFERENTE</t>
-        </is>
-      </c>
-      <c r="F93" t="n">
-        <v>200.02</v>
-      </c>
-      <c r="G93" t="n">
-        <v>0</v>
-      </c>
-      <c r="H93" t="n">
-        <v>-1750.95</v>
-      </c>
-      <c r="I93" t="n">
-        <v>0</v>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>Rafa</t>
-        </is>
-      </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L93" t="n">
-        <v>438009004</v>
-      </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N93" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P93" t="inlineStr">
-        <is>
-          <t>409122518/01</t>
-        </is>
-      </c>
-      <c r="Q93" t="inlineStr"/>
-    </row>
-    <row r="94">
-      <c r="A94" s="2" t="n">
-        <v>45694</v>
-      </c>
-      <c r="B94" t="n">
-        <v>5104345</v>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Compensación Anticipo 509011773/1</t>
-        </is>
-      </c>
-      <c r="D94" t="n">
-        <v>9004</v>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>CLIENTE PREFERENTE</t>
-        </is>
-      </c>
-      <c r="F94" t="n">
-        <v>30.71</v>
-      </c>
-      <c r="G94" t="n">
-        <v>0</v>
-      </c>
-      <c r="H94" t="n">
-        <v>-1750.95</v>
-      </c>
-      <c r="I94" t="n">
-        <v>0</v>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>M.Jose</t>
-        </is>
-      </c>
-      <c r="K94" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="L94" t="n">
-        <v>438009004</v>
-      </c>
-      <c r="M94" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="N94" t="inlineStr">
-        <is>
-          <t>N</t>
-        </is>
-      </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="P94" t="inlineStr">
-        <is>
-          <t>509011773/1</t>
-        </is>
-      </c>
-      <c r="Q94" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>